<commit_message>
called dcf_sim function and printed results
</commit_message>
<xml_diff>
--- a/Portfolio_monte_carlo.xlsx
+++ b/Portfolio_monte_carlo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randycastleman/Dropbox/Code/Monte_Carlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randycastleman/local_code/monte_carlo_sim/monte_carlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBF0D59-C6A5-F247-95E7-5BFE2DFC9D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350DA6D-5E11-C74E-BFF2-7E29034B968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="680" windowWidth="23140" windowHeight="17080" xr2:uid="{530A2142-8305-FD44-BBA1-764568661865}"/>
+    <workbookView xWindow="1720" yWindow="580" windowWidth="21900" windowHeight="15660" xr2:uid="{530A2142-8305-FD44-BBA1-764568661865}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -126,8 +126,8 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="0.0\ \x"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0\ \x"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -292,16 +292,16 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -316,19 +316,19 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -656,7 +656,7 @@
   <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,7 +816,7 @@
         <v>-10</v>
       </c>
       <c r="D16" s="17">
-        <v>42.631924027114813</v>
+        <v>5</v>
       </c>
       <c r="E16" s="10">
         <v>45697</v>
@@ -830,11 +830,11 @@
       </c>
       <c r="H16" s="19">
         <f>D16/-C16</f>
-        <v>4.2631924027114811</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="21">
         <f>XIRR(C16:D16,E16:F16)</f>
-        <v>0.34536928534507749</v>
+        <v>-0.1322185907512903</v>
       </c>
       <c r="K16" s="20">
         <f>G16/365</f>
@@ -852,7 +852,7 @@
         <v>-10</v>
       </c>
       <c r="D17" s="17">
-        <v>20.022150617723575</v>
+        <v>5</v>
       </c>
       <c r="E17" s="10">
         <v>45738</v>
@@ -866,11 +866,11 @@
       </c>
       <c r="H17" s="19">
         <f>D17/-C17</f>
-        <v>2.0022150617723575</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="21">
         <f>XIRR(C17:D17,E17:F17)</f>
-        <v>0.38852481245994575</v>
+        <v>-0.27943421080708503</v>
       </c>
       <c r="K17" s="20">
         <f>G17/365</f>
@@ -986,7 +986,7 @@
       </c>
       <c r="D26" s="11">
         <f>SUM(D16:D25)</f>
-        <v>62.654074644838389</v>
+        <v>10</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="C28" s="30">
         <f>D26/-C26</f>
-        <v>3.1327037322419193</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="C29" s="31">
         <f>XIRR(C16:D25,E16:F25)</f>
-        <v>0.35837205052375798</v>
+        <v>-0.17225068770349025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Excel to gitignore?
</commit_message>
<xml_diff>
--- a/Portfolio_monte_carlo.xlsx
+++ b/Portfolio_monte_carlo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randycastleman/local_code/monte_carlo_sim/monte_carlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randycastleman/Dropbox/Mac/Documents/local_code/monte_carlo_sim/monte_carlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F350DA6D-5E11-C74E-BFF2-7E29034B968A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9E22E-0108-0E4F-8777-A39BA372C20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="580" windowWidth="21900" windowHeight="15660" xr2:uid="{530A2142-8305-FD44-BBA1-764568661865}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Fund Size</t>
   </si>
@@ -129,7 +129,7 @@
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.0\ \x"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -182,12 +182,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -203,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -220,15 +214,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -236,7 +221,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -292,36 +277,15 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -329,6 +293,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="168" fontId="6" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -656,7 +635,7 @@
   <dimension ref="B2:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,31 +795,32 @@
         <v>-10</v>
       </c>
       <c r="D16" s="17">
-        <v>5</v>
+        <v>60.818189750962262</v>
       </c>
       <c r="E16" s="10">
-        <v>45697</v>
+        <v>44657</v>
       </c>
       <c r="F16" s="10">
-        <v>47481</v>
+        <v>45935</v>
       </c>
       <c r="G16" s="25">
         <f>F16-E16</f>
-        <v>1784</v>
-      </c>
-      <c r="H16" s="19">
+        <v>1278</v>
+      </c>
+      <c r="H16" s="26">
         <f>D16/-C16</f>
-        <v>0.5</v>
-      </c>
-      <c r="I16" s="21">
+        <v>6.0818189750962262</v>
+      </c>
+      <c r="I16" s="27">
         <f>XIRR(C16:D16,E16:F16)</f>
-        <v>-0.1322185907512903</v>
-      </c>
-      <c r="K16" s="20">
+        <v>0.67464180588722233</v>
+      </c>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29">
         <f>G16/365</f>
-        <v>4.8876712328767127</v>
-      </c>
-      <c r="L16" s="3" t="s">
+        <v>3.5013698630136987</v>
+      </c>
+      <c r="L16" s="28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -852,31 +832,32 @@
         <v>-10</v>
       </c>
       <c r="D17" s="17">
-        <v>5</v>
+        <v>33.200678721027053</v>
       </c>
       <c r="E17" s="10">
-        <v>45738</v>
+        <v>45342</v>
       </c>
       <c r="F17" s="10">
-        <v>46510</v>
+        <v>46719</v>
       </c>
       <c r="G17" s="25">
         <f>F17-E17</f>
-        <v>772</v>
-      </c>
-      <c r="H17" s="19">
+        <v>1377</v>
+      </c>
+      <c r="H17" s="26">
         <f>D17/-C17</f>
-        <v>0.5</v>
-      </c>
-      <c r="I17" s="21">
+        <v>3.3200678721027055</v>
+      </c>
+      <c r="I17" s="27">
         <f>XIRR(C17:D17,E17:F17)</f>
-        <v>-0.27943421080708503</v>
-      </c>
-      <c r="K17" s="20">
+        <v>0.37448466420173643</v>
+      </c>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29">
         <f>G17/365</f>
-        <v>2.1150684931506851</v>
-      </c>
-      <c r="L17" s="3" t="s">
+        <v>3.7726027397260276</v>
+      </c>
+      <c r="L17" s="28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -884,97 +865,297 @@
       <c r="B18" s="1">
         <v>3</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="21"/>
+      <c r="C18" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D18" s="5">
+        <v>54.558458729276964</v>
+      </c>
+      <c r="E18" s="9">
+        <v>45218</v>
+      </c>
+      <c r="F18" s="9">
+        <v>47067</v>
+      </c>
+      <c r="G18" s="25">
+        <f t="shared" ref="G18:G25" si="0">F18-E18</f>
+        <v>1849</v>
+      </c>
+      <c r="H18" s="26">
+        <f t="shared" ref="H18:H25" si="1">D18/-C18</f>
+        <v>5.4558458729276964</v>
+      </c>
+      <c r="I18" s="27">
+        <f t="shared" ref="I18:I25" si="2">XIRR(C18:D18,E18:F18)</f>
+        <v>0.3978466331958771</v>
+      </c>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29">
+        <f t="shared" ref="K18:K25" si="3">G18/365</f>
+        <v>5.065753424657534</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>4</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="21"/>
+      <c r="C19" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D19" s="5">
+        <v>47.562368214877829</v>
+      </c>
+      <c r="E19" s="9">
+        <v>45297</v>
+      </c>
+      <c r="F19" s="9">
+        <v>47347</v>
+      </c>
+      <c r="G19" s="25">
+        <f t="shared" si="0"/>
+        <v>2050</v>
+      </c>
+      <c r="H19" s="26">
+        <f t="shared" si="1"/>
+        <v>4.756236821487783</v>
+      </c>
+      <c r="I19" s="27">
+        <f t="shared" si="2"/>
+        <v>0.32003648877143875</v>
+      </c>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29">
+        <f t="shared" si="3"/>
+        <v>5.6164383561643838</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>5</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="21"/>
+      <c r="C20" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D20" s="5">
+        <v>12.485479555985119</v>
+      </c>
+      <c r="E20" s="9">
+        <v>46069</v>
+      </c>
+      <c r="F20" s="9">
+        <v>48002</v>
+      </c>
+      <c r="G20" s="25">
+        <f t="shared" si="0"/>
+        <v>1933</v>
+      </c>
+      <c r="H20" s="26">
+        <f t="shared" si="1"/>
+        <v>1.2485479555985119</v>
+      </c>
+      <c r="I20" s="27">
+        <f t="shared" si="2"/>
+        <v>4.2806622385978696E-2</v>
+      </c>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29">
+        <f t="shared" si="3"/>
+        <v>5.2958904109589042</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="21"/>
+      <c r="C21" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D21" s="5">
+        <v>20.993781035688926</v>
+      </c>
+      <c r="E21" s="9">
+        <v>45708</v>
+      </c>
+      <c r="F21" s="9">
+        <v>48566</v>
+      </c>
+      <c r="G21" s="25">
+        <f t="shared" si="0"/>
+        <v>2858</v>
+      </c>
+      <c r="H21" s="26">
+        <f t="shared" si="1"/>
+        <v>2.0993781035688928</v>
+      </c>
+      <c r="I21" s="27">
+        <f t="shared" si="2"/>
+        <v>9.9346858263015758E-2</v>
+      </c>
+      <c r="J21" s="28"/>
+      <c r="K21" s="29">
+        <f t="shared" si="3"/>
+        <v>7.8301369863013699</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>7</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="21"/>
+      <c r="C22" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D22" s="5">
+        <v>14.313961769104877</v>
+      </c>
+      <c r="E22" s="9">
+        <v>46308</v>
+      </c>
+      <c r="F22" s="9">
+        <v>47481</v>
+      </c>
+      <c r="G22" s="25">
+        <f t="shared" si="0"/>
+        <v>1173</v>
+      </c>
+      <c r="H22" s="26">
+        <f t="shared" si="1"/>
+        <v>1.4313961769104877</v>
+      </c>
+      <c r="I22" s="27">
+        <f t="shared" si="2"/>
+        <v>0.11806607842445374</v>
+      </c>
+      <c r="J22" s="28"/>
+      <c r="K22" s="29">
+        <f t="shared" si="3"/>
+        <v>3.2136986301369861</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>8</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="21"/>
+      <c r="C23" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D23" s="5">
+        <v>16.252687746912379</v>
+      </c>
+      <c r="E23" s="9">
+        <v>45317</v>
+      </c>
+      <c r="F23" s="9">
+        <v>47065</v>
+      </c>
+      <c r="G23" s="25">
+        <f t="shared" si="0"/>
+        <v>1748</v>
+      </c>
+      <c r="H23" s="26">
+        <f t="shared" si="1"/>
+        <v>1.625268774691238</v>
+      </c>
+      <c r="I23" s="27">
+        <f t="shared" si="2"/>
+        <v>0.10673412680625918</v>
+      </c>
+      <c r="J23" s="28"/>
+      <c r="K23" s="29">
+        <f t="shared" si="3"/>
+        <v>4.7890410958904113</v>
+      </c>
+      <c r="L23" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>9</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="21"/>
+      <c r="C24" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D24" s="5">
+        <v>63.437260825403698</v>
+      </c>
+      <c r="E24" s="9">
+        <v>45562</v>
+      </c>
+      <c r="F24" s="9">
+        <v>48522</v>
+      </c>
+      <c r="G24" s="25">
+        <f t="shared" si="0"/>
+        <v>2960</v>
+      </c>
+      <c r="H24" s="26">
+        <f t="shared" si="1"/>
+        <v>6.3437260825403694</v>
+      </c>
+      <c r="I24" s="27">
+        <f t="shared" si="2"/>
+        <v>0.25584991574287408</v>
+      </c>
+      <c r="J24" s="28"/>
+      <c r="K24" s="29">
+        <f t="shared" si="3"/>
+        <v>8.1095890410958908</v>
+      </c>
+      <c r="L24" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>10</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="28"/>
+      <c r="C25" s="5">
+        <v>-10</v>
+      </c>
+      <c r="D25" s="5">
+        <v>6.6026500400554813</v>
+      </c>
+      <c r="E25" s="9">
+        <v>45379</v>
+      </c>
+      <c r="F25" s="9">
+        <v>47589</v>
+      </c>
+      <c r="G25" s="25">
+        <f t="shared" si="0"/>
+        <v>2210</v>
+      </c>
+      <c r="H25" s="26">
+        <f t="shared" si="1"/>
+        <v>0.66026500400554811</v>
+      </c>
+      <c r="I25" s="27">
+        <f t="shared" si="2"/>
+        <v>-6.6262146830558769E-2</v>
+      </c>
+      <c r="J25" s="28"/>
+      <c r="K25" s="29">
+        <f t="shared" si="3"/>
+        <v>6.0547945205479454</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -982,36 +1163,36 @@
       </c>
       <c r="C26" s="11">
         <f>SUM(C16:C25)</f>
-        <v>-20</v>
+        <v>-100</v>
       </c>
       <c r="D26" s="11">
         <f>SUM(D16:D25)</f>
-        <v>10</v>
+        <v>330.22551638929463</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="23">
         <f>D26/-C26</f>
-        <v>0.5</v>
+        <v>3.302255163892946</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="31">
+      <c r="C29" s="24">
         <f>XIRR(C16:D25,E16:F25)</f>
-        <v>-0.17225068770349025</v>
+        <v>0.31359677910804751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ignore to add Excel and temp Excel file names
</commit_message>
<xml_diff>
--- a/Portfolio_monte_carlo.xlsx
+++ b/Portfolio_monte_carlo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randycastleman/Dropbox/Mac/Documents/local_code/monte_carlo_sim/monte_carlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F9E22E-0108-0E4F-8777-A39BA372C20D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C8D1BF-FD4B-8647-95DB-11955A72023B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1720" yWindow="580" windowWidth="21900" windowHeight="15660" xr2:uid="{530A2142-8305-FD44-BBA1-764568661865}"/>
   </bookViews>
@@ -795,30 +795,30 @@
         <v>-10</v>
       </c>
       <c r="D16" s="17">
-        <v>60.818189750962262</v>
+        <v>35.993671079192097</v>
       </c>
       <c r="E16" s="10">
-        <v>44657</v>
+        <v>45712</v>
       </c>
       <c r="F16" s="10">
-        <v>45935</v>
+        <v>47115</v>
       </c>
       <c r="G16" s="25">
         <f>F16-E16</f>
-        <v>1278</v>
+        <v>1403</v>
       </c>
       <c r="H16" s="26">
         <f>D16/-C16</f>
-        <v>6.0818189750962262</v>
+        <v>3.5993671079192096</v>
       </c>
       <c r="I16" s="27">
         <f>XIRR(C16:D16,E16:F16)</f>
-        <v>0.67464180588722233</v>
+        <v>0.39542345404624946</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="29">
         <f>G16/365</f>
-        <v>3.5013698630136987</v>
+        <v>3.8438356164383563</v>
       </c>
       <c r="L16" s="28" t="s">
         <v>25</v>
@@ -832,30 +832,30 @@
         <v>-10</v>
       </c>
       <c r="D17" s="17">
-        <v>33.200678721027053</v>
+        <v>268.76625466002241</v>
       </c>
       <c r="E17" s="10">
-        <v>45342</v>
+        <v>45334</v>
       </c>
       <c r="F17" s="10">
-        <v>46719</v>
+        <v>47533</v>
       </c>
       <c r="G17" s="25">
         <f>F17-E17</f>
-        <v>1377</v>
+        <v>2199</v>
       </c>
       <c r="H17" s="26">
         <f>D17/-C17</f>
-        <v>3.3200678721027055</v>
+        <v>26.876625466002242</v>
       </c>
       <c r="I17" s="27">
         <f>XIRR(C17:D17,E17:F17)</f>
-        <v>0.37448466420173643</v>
+        <v>0.72684797048568739</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="29">
         <f>G17/365</f>
-        <v>3.7726027397260276</v>
+        <v>6.0246575342465754</v>
       </c>
       <c r="L17" s="28" t="s">
         <v>25</v>
@@ -869,30 +869,30 @@
         <v>-10</v>
       </c>
       <c r="D18" s="5">
-        <v>54.558458729276964</v>
+        <v>107.45787495594396</v>
       </c>
       <c r="E18" s="9">
-        <v>45218</v>
+        <v>45762</v>
       </c>
       <c r="F18" s="9">
-        <v>47067</v>
+        <v>47648</v>
       </c>
       <c r="G18" s="25">
         <f t="shared" ref="G18:G25" si="0">F18-E18</f>
-        <v>1849</v>
+        <v>1886</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" ref="H18:H25" si="1">D18/-C18</f>
-        <v>5.4558458729276964</v>
+        <v>10.745787495594396</v>
       </c>
       <c r="I18" s="27">
         <f t="shared" ref="I18:I25" si="2">XIRR(C18:D18,E18:F18)</f>
-        <v>0.3978466331958771</v>
+        <v>0.58334975838661196</v>
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="29">
         <f t="shared" ref="K18:K25" si="3">G18/365</f>
-        <v>5.065753424657534</v>
+        <v>5.1671232876712327</v>
       </c>
       <c r="L18" s="28" t="s">
         <v>25</v>
@@ -906,30 +906,30 @@
         <v>-10</v>
       </c>
       <c r="D19" s="5">
-        <v>47.562368214877829</v>
+        <v>17.583127519126556</v>
       </c>
       <c r="E19" s="9">
-        <v>45297</v>
+        <v>45236</v>
       </c>
       <c r="F19" s="9">
-        <v>47347</v>
+        <v>46337</v>
       </c>
       <c r="G19" s="25">
         <f t="shared" si="0"/>
-        <v>2050</v>
+        <v>1101</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" si="1"/>
-        <v>4.756236821487783</v>
+        <v>1.7583127519126556</v>
       </c>
       <c r="I19" s="27">
         <f t="shared" si="2"/>
-        <v>0.32003648877143875</v>
+        <v>0.20573949217796328</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="29">
         <f t="shared" si="3"/>
-        <v>5.6164383561643838</v>
+        <v>3.0164383561643837</v>
       </c>
       <c r="L19" s="28" t="s">
         <v>25</v>
@@ -943,30 +943,30 @@
         <v>-10</v>
       </c>
       <c r="D20" s="5">
-        <v>12.485479555985119</v>
+        <v>101.54818637999711</v>
       </c>
       <c r="E20" s="9">
-        <v>46069</v>
+        <v>45860</v>
       </c>
       <c r="F20" s="9">
-        <v>48002</v>
+        <v>47917</v>
       </c>
       <c r="G20" s="25">
         <f t="shared" si="0"/>
-        <v>1933</v>
+        <v>2057</v>
       </c>
       <c r="H20" s="26">
         <f t="shared" si="1"/>
-        <v>1.2485479555985119</v>
+        <v>10.154818637999711</v>
       </c>
       <c r="I20" s="27">
         <f t="shared" si="2"/>
-        <v>4.2806622385978696E-2</v>
+        <v>0.50878308415412898</v>
       </c>
       <c r="J20" s="28"/>
       <c r="K20" s="29">
         <f t="shared" si="3"/>
-        <v>5.2958904109589042</v>
+        <v>5.6356164383561644</v>
       </c>
       <c r="L20" s="28" t="s">
         <v>25</v>
@@ -980,30 +980,30 @@
         <v>-10</v>
       </c>
       <c r="D21" s="5">
-        <v>20.993781035688926</v>
+        <v>137.471168681488</v>
       </c>
       <c r="E21" s="9">
-        <v>45708</v>
+        <v>45825</v>
       </c>
       <c r="F21" s="9">
-        <v>48566</v>
+        <v>48239</v>
       </c>
       <c r="G21" s="25">
         <f t="shared" si="0"/>
-        <v>2858</v>
+        <v>2414</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" si="1"/>
-        <v>2.0993781035688928</v>
+        <v>13.747116868148799</v>
       </c>
       <c r="I21" s="27">
         <f t="shared" si="2"/>
-        <v>9.9346858263015758E-2</v>
+        <v>0.48627477288246157</v>
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="29">
         <f t="shared" si="3"/>
-        <v>7.8301369863013699</v>
+        <v>6.6136986301369864</v>
       </c>
       <c r="L21" s="28" t="s">
         <v>25</v>
@@ -1017,30 +1017,30 @@
         <v>-10</v>
       </c>
       <c r="D22" s="5">
-        <v>14.313961769104877</v>
+        <v>210.13320332399107</v>
       </c>
       <c r="E22" s="9">
-        <v>46308</v>
+        <v>45759</v>
       </c>
       <c r="F22" s="9">
-        <v>47481</v>
+        <v>47754</v>
       </c>
       <c r="G22" s="25">
         <f t="shared" si="0"/>
-        <v>1173</v>
+        <v>1995</v>
       </c>
       <c r="H22" s="26">
         <f t="shared" si="1"/>
-        <v>1.4313961769104877</v>
+        <v>21.013320332399108</v>
       </c>
       <c r="I22" s="27">
         <f t="shared" si="2"/>
-        <v>0.11806607842445374</v>
+        <v>0.74566208124160749</v>
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="29">
         <f t="shared" si="3"/>
-        <v>3.2136986301369861</v>
+        <v>5.4657534246575343</v>
       </c>
       <c r="L22" s="28" t="s">
         <v>25</v>
@@ -1054,30 +1054,30 @@
         <v>-10</v>
       </c>
       <c r="D23" s="5">
-        <v>16.252687746912379</v>
+        <v>7.4955300174986341</v>
       </c>
       <c r="E23" s="9">
-        <v>45317</v>
+        <v>45512</v>
       </c>
       <c r="F23" s="9">
-        <v>47065</v>
+        <v>48605</v>
       </c>
       <c r="G23" s="25">
         <f t="shared" si="0"/>
-        <v>1748</v>
+        <v>3093</v>
       </c>
       <c r="H23" s="26">
         <f t="shared" si="1"/>
-        <v>1.625268774691238</v>
+        <v>0.74955300174986339</v>
       </c>
       <c r="I23" s="27">
         <f t="shared" si="2"/>
-        <v>0.10673412680625918</v>
+        <v>-3.3447107672691351E-2</v>
       </c>
       <c r="J23" s="28"/>
       <c r="K23" s="29">
         <f t="shared" si="3"/>
-        <v>4.7890410958904113</v>
+        <v>8.4739726027397264</v>
       </c>
       <c r="L23" s="28" t="s">
         <v>25</v>
@@ -1091,30 +1091,30 @@
         <v>-10</v>
       </c>
       <c r="D24" s="5">
-        <v>63.437260825403698</v>
+        <v>64.264035171550873</v>
       </c>
       <c r="E24" s="9">
-        <v>45562</v>
+        <v>45008</v>
       </c>
       <c r="F24" s="9">
-        <v>48522</v>
+        <v>47205</v>
       </c>
       <c r="G24" s="25">
         <f t="shared" si="0"/>
-        <v>2960</v>
+        <v>2197</v>
       </c>
       <c r="H24" s="26">
         <f t="shared" si="1"/>
-        <v>6.3437260825403694</v>
+        <v>6.4264035171550873</v>
       </c>
       <c r="I24" s="27">
         <f t="shared" si="2"/>
-        <v>0.25584991574287408</v>
+        <v>0.36217303872108475</v>
       </c>
       <c r="J24" s="28"/>
       <c r="K24" s="29">
         <f t="shared" si="3"/>
-        <v>8.1095890410958908</v>
+        <v>6.0191780821917806</v>
       </c>
       <c r="L24" s="28" t="s">
         <v>25</v>
@@ -1128,30 +1128,30 @@
         <v>-10</v>
       </c>
       <c r="D25" s="5">
-        <v>6.6026500400554813</v>
+        <v>35.251036294235412</v>
       </c>
       <c r="E25" s="9">
-        <v>45379</v>
+        <v>45946</v>
       </c>
       <c r="F25" s="9">
-        <v>47589</v>
+        <v>47911</v>
       </c>
       <c r="G25" s="25">
         <f t="shared" si="0"/>
-        <v>2210</v>
+        <v>1965</v>
       </c>
       <c r="H25" s="26">
         <f t="shared" si="1"/>
-        <v>0.66026500400554811</v>
+        <v>3.5251036294235414</v>
       </c>
       <c r="I25" s="27">
         <f t="shared" si="2"/>
-        <v>-6.6262146830558769E-2</v>
+        <v>0.26368120312690735</v>
       </c>
       <c r="J25" s="28"/>
       <c r="K25" s="29">
         <f t="shared" si="3"/>
-        <v>6.0547945205479454</v>
+        <v>5.3835616438356162</v>
       </c>
       <c r="L25" s="28" t="s">
         <v>25</v>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="D26" s="11">
         <f>SUM(D16:D25)</f>
-        <v>330.22551638929463</v>
+        <v>985.96408808304614</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="C28" s="23">
         <f>D26/-C26</f>
-        <v>3.302255163892946</v>
+        <v>9.8596408808304616</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="C29" s="24">
         <f>XIRR(C16:D25,E16:F25)</f>
-        <v>0.31359677910804751</v>
+        <v>0.49625533223152152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>